<commit_message>
Nuevos experimentos problemas lineales?
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9_1_1/compare/C-Estacionario/ex9_1_1_C-Estacionario.xlsx
+++ b/experiment/linear/ex9_1_1/compare/C-Estacionario/ex9_1_1_C-Estacionario.xlsx
@@ -494,13 +494,13 @@
         <v>0.0</v>
       </c>
       <c r="E2">
-        <v>0.000241233</v>
+        <v>0.00021951</v>
       </c>
       <c r="F2">
-        <v>0.016033918</v>
+        <v>0.01400598</v>
       </c>
       <c r="G2">
-        <v>0.0004499973887</v>
+        <v>0.00039225899699999996</v>
       </c>
       <c r="H2">
         <v>1973</v>
@@ -532,13 +532,13 @@
         <v>0.0</v>
       </c>
       <c r="E3">
-        <v>0.002363885</v>
+        <v>0.00196704</v>
       </c>
       <c r="F3">
-        <v>0.007391571</v>
+        <v>0.01721106</v>
       </c>
       <c r="G3">
-        <v>0.003066476192874693</v>
+        <v>0.0024532412727272727</v>
       </c>
       <c r="H3">
         <v>2331</v>
@@ -570,13 +570,13 @@
         <v>0.0</v>
       </c>
       <c r="E4">
-        <v>0.004928141</v>
+        <v>0.00419832</v>
       </c>
       <c r="F4">
-        <v>0.010186458</v>
+        <v>0.16120332</v>
       </c>
       <c r="G4">
-        <v>0.005898166218064516</v>
+        <v>0.005188931775700934</v>
       </c>
       <c r="H4">
         <v>6448</v>

</xml_diff>

<commit_message>
Fix background and migrate to new template
</commit_message>
<xml_diff>
--- a/experiment/linear/ex9_1_1/compare/C-Estacionario/ex9_1_1_C-Estacionario.xlsx
+++ b/experiment/linear/ex9_1_1/compare/C-Estacionario/ex9_1_1_C-Estacionario.xlsx
@@ -488,13 +488,13 @@
         <v>0.0</v>
       </c>
       <c r="E2">
-        <v>0.000287505</v>
+        <v>0.000246323</v>
       </c>
       <c r="F2">
-        <v>0.023282776</v>
+        <v>0.016120654</v>
       </c>
       <c r="G2">
-        <v>0.000635000454568625</v>
+        <v>0.0004682440455</v>
       </c>
       <c r="H2">
         <v>1976</v>
@@ -526,13 +526,13 @@
         <v>-27.94109615193122</v>
       </c>
       <c r="E3">
-        <v>0.007851779</v>
+        <v>0.009391366</v>
       </c>
       <c r="F3">
-        <v>0.034480998</v>
+        <v>0.015660926</v>
       </c>
       <c r="G3">
-        <v>0.00990405125148515</v>
+        <v>0.01053818123628692</v>
       </c>
       <c r="H3">
         <v>6656</v>

</xml_diff>